<commit_message>
Added Roslyn Model and Test Resul
</commit_message>
<xml_diff>
--- a/Model/Results.xlsx
+++ b/Model/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Workbrench\GitHub_NeturalNetworks\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D7ECB2-19CA-4311-A2BE-733F0BAC67B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037A76C-9C2A-4185-A155-3B7517B9C5CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E72B3458-5A66-4407-99B4-AD0E89C04A48}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>Features</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Title + Description</t>
   </si>
   <si>
-    <t>Epochs(=30)</t>
-  </si>
-  <si>
     <t>Train/Test Data (80/20)</t>
   </si>
   <si>
@@ -71,6 +68,12 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>Epochs(=30-60)</t>
+  </si>
+  <si>
+    <t>corefx</t>
   </si>
 </sst>
 </file>
@@ -126,8 +129,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E65EC3BA-3B0C-42CA-A1C3-8CB515A6DD64}" name="Table2" displayName="Table2" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{232B8648-183D-412B-B8DA-58BCBCD3A254}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E65EC3BA-3B0C-42CA-A1C3-8CB515A6DD64}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0">
+  <autoFilter ref="A1:F7" xr:uid="{232B8648-183D-412B-B8DA-58BCBCD3A254}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{87D59A98-1961-4BD2-8DBE-009A0CE33A9F}" name="Datasets"/>
     <tableColumn id="2" xr3:uid="{A42F7268-252A-431F-858D-E499EBB1319F}" name="Features"/>
@@ -452,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEC94D7-4942-4B2E-BF27-38361FE3719D}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -509,7 +512,7 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -529,19 +532,56 @@
         <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -558,7 +598,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +651,7 @@
         <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -631,20 +671,44 @@
         <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
datasets, model check in
</commit_message>
<xml_diff>
--- a/Model/Results.xlsx
+++ b/Model/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Workbrench\GitHub_NeturalNetworks\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037A76C-9C2A-4185-A155-3B7517B9C5CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ABCA68-D609-4651-A4BA-F5A96512AA85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E72B3458-5A66-4407-99B4-AD0E89C04A48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E72B3458-5A66-4407-99B4-AD0E89C04A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Prediction Results" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Features</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Accuracy</t>
   </si>
   <si>
-    <t>SVF</t>
-  </si>
-  <si>
     <t xml:space="preserve">Title </t>
   </si>
   <si>
@@ -64,16 +61,46 @@
     <t>Train/Test Data (80/20)</t>
   </si>
   <si>
-    <t>Roslyn</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
-    <t>Epochs(=30-60)</t>
-  </si>
-  <si>
-    <t>corefx</t>
+    <t>Epochs(=60)</t>
+  </si>
+  <si>
+    <t>SVF (Single Label associated with a Issue)</t>
+  </si>
+  <si>
+    <t>SVF (Multiple Labels associated with a Issue)</t>
+  </si>
+  <si>
+    <t>corefx (Multiple Labels associated with a Issue)</t>
+  </si>
+  <si>
+    <t>corefx (Single Label associated with a Issue)</t>
+  </si>
+  <si>
+    <t>Roslyn (Multiple Labels associated with a Issue)</t>
+  </si>
+  <si>
+    <t>Roslyn (Single Label associated with a Issue)</t>
+  </si>
+  <si>
+    <t>SVF  (Multiple Assignee/Contributors associated with a Issue)</t>
+  </si>
+  <si>
+    <t>SVF  (Single Assignee/Contributor associated with a Issue)</t>
+  </si>
+  <si>
+    <t>Roslyn (Multiple Assignee/Contributors associated with a Issue)</t>
+  </si>
+  <si>
+    <t>Roslyn (Single Assignee/Contributor associated with a Issue)</t>
+  </si>
+  <si>
+    <t>corefx (Multiple Assignee/Contributor associated with a Issue)</t>
+  </si>
+  <si>
+    <t>corefx (Single Assignee/Contributor associated with a Issue)</t>
   </si>
 </sst>
 </file>
@@ -129,8 +156,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E65EC3BA-3B0C-42CA-A1C3-8CB515A6DD64}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{232B8648-183D-412B-B8DA-58BCBCD3A254}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E65EC3BA-3B0C-42CA-A1C3-8CB515A6DD64}" name="Table2" displayName="Table2" ref="A1:F13" totalsRowShown="0">
+  <autoFilter ref="A1:F13" xr:uid="{232B8648-183D-412B-B8DA-58BCBCD3A254}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{87D59A98-1961-4BD2-8DBE-009A0CE33A9F}" name="Datasets"/>
     <tableColumn id="2" xr3:uid="{A42F7268-252A-431F-858D-E499EBB1319F}" name="Features"/>
@@ -144,8 +171,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FD2B22C-1B90-4061-A84E-38DF663A2912}" name="Table1" displayName="Table1" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{27811E21-0D68-404E-BC12-27AD40B9440E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FD2B22C-1B90-4061-A84E-38DF663A2912}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0">
+  <autoFilter ref="A1:F13" xr:uid="{27811E21-0D68-404E-BC12-27AD40B9440E}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CA0C908E-90FA-45C5-9A9D-F7D56E051B6B}" name="Datasets"/>
     <tableColumn id="2" xr3:uid="{E82A6512-4140-4220-A305-17D6E5E0AC2F}" name="Features"/>
@@ -455,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEC94D7-4942-4B2E-BF27-38361FE3719D}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
@@ -494,30 +521,30 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>33</v>
       </c>
       <c r="E2">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -532,57 +559,144 @@
         <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -595,19 +709,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B78A8AA-B1C2-471B-B616-6AEBED967801}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -633,10 +746,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -651,12 +764,12 @@
         <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -671,44 +784,132 @@
         <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>47</v>
+      </c>
+      <c r="F5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check-in Roslyn 2019 issues downloaded
</commit_message>
<xml_diff>
--- a/Model/Results.xlsx
+++ b/Model/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Workbrench\GitHub_NeturalNetworks\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ABCA68-D609-4651-A4BA-F5A96512AA85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C3F94A-DE1A-4798-B40B-7C57E932A8FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E72B3458-5A66-4407-99B4-AD0E89C04A48}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{E72B3458-5A66-4407-99B4-AD0E89C04A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Prediction Results" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>Features</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>corefx (Single Assignee/Contributor associated with a Issue)</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Roslyn  - Total Assignee OR Contributors = 15</t>
+  </si>
+  <si>
+    <t>SVF  - Total Assignee OR Contributors = 7</t>
   </si>
 </sst>
 </file>
@@ -124,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,17 +141,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -182,6 +219,16 @@
     <tableColumn id="6" xr3:uid="{5C9F49E0-EFBE-4E9C-BB80-A6C1A5CEF6BC}" name="Accuracy"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{579B72C5-E85C-44FF-B683-BF6D98A31DDF}" name="Table3" displayName="Table3" ref="H2:H6" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="H2:H6" xr:uid="{4D5B3ED1-3D7F-4251-9A31-831089A64FE5}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{C880BEB9-9FC9-4B08-B2CE-C627ED833672}" name="Test Data"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -712,7 +759,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +769,7 @@
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,8 +811,8 @@
       <c r="F2">
         <v>75</v>
       </c>
-      <c r="H2" t="s">
-        <v>10</v>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -783,8 +831,8 @@
       <c r="F3">
         <v>75</v>
       </c>
-      <c r="H3" t="s">
-        <v>8</v>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,6 +854,9 @@
       <c r="F4">
         <v>89</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -822,6 +873,9 @@
       </c>
       <c r="F5">
         <v>89</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -843,6 +897,9 @@
       <c r="F6">
         <v>6</v>
       </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -885,6 +942,18 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -914,8 +983,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>